<commit_message>
Large addition, class constructed, epochs implemented, two models added.
</commit_message>
<xml_diff>
--- a/Metadata - Gathered data/relationsheet_kinship_detection (version 1).xlsb.xlsx
+++ b/Metadata - Gathered data/relationsheet_kinship_detection (version 1).xlsb.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="86">
   <si>
     <t>Path</t>
   </si>
@@ -87,7 +87,7 @@
     <t>0</t>
   </si>
   <si>
-    <t>4-1</t>
+    <t>1-4</t>
   </si>
   <si>
     <t>1-2, 1-3</t>
@@ -114,105 +114,99 @@
     <t>40/2</t>
   </si>
   <si>
-    <t>2-4</t>
+    <t>4-2</t>
   </si>
   <si>
     <t xml:space="preserve"> 2-3</t>
   </si>
   <si>
+    <t>1-2</t>
+  </si>
+  <si>
+    <t>26 to 40</t>
+  </si>
+  <si>
+    <t>prince harry</t>
+  </si>
+  <si>
+    <t>40-3</t>
+  </si>
+  <si>
+    <t>40/3</t>
+  </si>
+  <si>
+    <t>4-3</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>1-3</t>
+  </si>
+  <si>
+    <t>prince william</t>
+  </si>
+  <si>
+    <t>40-4</t>
+  </si>
+  <si>
+    <t>40/4</t>
+  </si>
+  <si>
+    <t>4-2,4-3</t>
+  </si>
+  <si>
+    <t>prince( now KING) Charles III</t>
+  </si>
+  <si>
+    <t>41-1</t>
+  </si>
+  <si>
+    <t>41/1</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>41 to 60</t>
+  </si>
+  <si>
+    <t>David Beckham</t>
+  </si>
+  <si>
+    <t>41-2</t>
+  </si>
+  <si>
+    <t>41/2</t>
+  </si>
+  <si>
+    <t>Victoria Beckham (His wife)</t>
+  </si>
+  <si>
+    <t>41-3</t>
+  </si>
+  <si>
+    <t>41/3</t>
+  </si>
+  <si>
+    <t>15 to 25</t>
+  </si>
+  <si>
+    <t>Brooklyn Beckham</t>
+  </si>
+  <si>
+    <t>42-1</t>
+  </si>
+  <si>
+    <t>42/1</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
     <t>2-1</t>
   </si>
   <si>
-    <t>26 to 40</t>
-  </si>
-  <si>
-    <t>prince harry</t>
-  </si>
-  <si>
-    <t>40-3</t>
-  </si>
-  <si>
-    <t>40/3</t>
-  </si>
-  <si>
-    <t>3-4</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 3-2</t>
-  </si>
-  <si>
-    <t>3-1</t>
-  </si>
-  <si>
-    <t>prince william</t>
-  </si>
-  <si>
-    <t>40-4</t>
-  </si>
-  <si>
-    <t>40/4</t>
-  </si>
-  <si>
-    <t>4-2,4-3</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1-4 </t>
-  </si>
-  <si>
-    <t>prince( now KING) Charles III</t>
-  </si>
-  <si>
-    <t>41-1</t>
-  </si>
-  <si>
-    <t>41/1</t>
-  </si>
-  <si>
-    <t>41</t>
-  </si>
-  <si>
-    <t>1-3</t>
-  </si>
-  <si>
-    <t>41 to 60</t>
-  </si>
-  <si>
-    <t>David Beckham</t>
-  </si>
-  <si>
-    <t>41-2</t>
-  </si>
-  <si>
-    <t>41/2</t>
-  </si>
-  <si>
-    <t>Victoria Beckham (His wife)</t>
-  </si>
-  <si>
-    <t>41-3</t>
-  </si>
-  <si>
-    <t>41/3</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 3-1</t>
-  </si>
-  <si>
-    <t>15 to 25</t>
-  </si>
-  <si>
-    <t>Brooklyn Beckham</t>
-  </si>
-  <si>
-    <t>42-1</t>
-  </si>
-  <si>
-    <t>42/1</t>
-  </si>
-  <si>
-    <t>42</t>
-  </si>
-  <si>
     <t>42 to 60</t>
   </si>
   <si>
@@ -231,9 +225,6 @@
     <t>42/2</t>
   </si>
   <si>
-    <t>1-2</t>
-  </si>
-  <si>
     <t>Martin Sheen</t>
   </si>
   <si>
@@ -264,7 +255,7 @@
     <t>43/2</t>
   </si>
   <si>
-    <t>2-1,2-3</t>
+    <t>1-2,2-3</t>
   </si>
   <si>
     <t>Liam Hemsworth</t>
@@ -276,7 +267,7 @@
     <t>43/3</t>
   </si>
   <si>
-    <t>3-1,3-2</t>
+    <t>1-3,2-3</t>
   </si>
   <si>
     <t>Chris Hemsworth</t>
@@ -697,7 +688,7 @@
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75" customFormat="1" s="13">
       <c r="A1" s="14" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -738,7 +729,7 @@
     <col min="20" max="20" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -984,7 +975,7 @@
         <v>42</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1" t="s">
         <v>43</v>
       </c>
@@ -1001,7 +992,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="G5" s="7"/>
       <c r="H5" s="4">
@@ -1041,21 +1032,21 @@
         <v>1</v>
       </c>
       <c r="T5" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+      <c r="A6" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="D6" s="2" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="E6" s="4">
         <v>0</v>
@@ -1088,7 +1079,7 @@
         <v>1</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="P6" s="1" t="s">
         <v>26</v>
@@ -1103,18 +1094,18 @@
         <v>1</v>
       </c>
       <c r="T6" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+      <c r="A7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="C7" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>22</v>
@@ -1148,7 +1139,7 @@
         <v>1</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="P7" s="1" t="s">
         <v>26</v>
@@ -1163,25 +1154,25 @@
         <v>1</v>
       </c>
       <c r="T7" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+      <c r="A8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="C8" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>41</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="3" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="G8" s="4">
         <v>0</v>
@@ -1208,7 +1199,7 @@
         <v>1</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="P8" s="1" t="s">
         <v>26</v>
@@ -1223,21 +1214,21 @@
         <v>1</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="E9" s="4">
         <v>0</v>
@@ -1270,36 +1261,36 @@
         <v>1</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="P9" s="8" t="s">
         <v>26</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="S9" s="4">
         <v>1</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E10" s="4">
         <v>0</v>
@@ -1338,27 +1329,27 @@
         <v>26</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="S10" s="4">
         <v>1</v>
       </c>
       <c r="T10" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>22</v>
@@ -1373,7 +1364,7 @@
         <v>0</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="I11" s="4">
         <v>0</v>
@@ -1400,27 +1391,27 @@
         <v>26</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="S11" s="4">
         <v>1</v>
       </c>
       <c r="T11" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>22</v>
@@ -1435,7 +1426,7 @@
         <v>0</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I12" s="4">
         <v>0</v>
@@ -1462,27 +1453,27 @@
         <v>26</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="S12" s="4">
         <v>1</v>
       </c>
       <c r="T12" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>22</v>
@@ -1497,7 +1488,7 @@
         <v>0</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="I13" s="4">
         <v>0</v>
@@ -1524,16 +1515,16 @@
         <v>26</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="S13" s="4">
         <v>1</v>
       </c>
       <c r="T13" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
@@ -1954,7 +1945,7 @@
       <c r="S32" s="6"/>
       <c r="T32" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
       <c r="A33" s="8"/>
       <c r="B33" s="8"/>
       <c r="C33" s="6"/>
@@ -1976,7 +1967,7 @@
       <c r="S33" s="6"/>
       <c r="T33" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
       <c r="A34" s="8"/>
       <c r="B34" s="8"/>
       <c r="C34" s="6"/>
@@ -1998,7 +1989,7 @@
       <c r="S34" s="6"/>
       <c r="T34" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
       <c r="A35" s="8"/>
       <c r="B35" s="8"/>
       <c r="C35" s="6"/>
@@ -2020,7 +2011,7 @@
       <c r="S35" s="6"/>
       <c r="T35" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
       <c r="C36" s="6"/>
@@ -2042,7 +2033,7 @@
       <c r="S36" s="6"/>
       <c r="T36" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
       <c r="A37" s="8"/>
       <c r="B37" s="8"/>
       <c r="C37" s="6"/>
@@ -2064,7 +2055,7 @@
       <c r="S37" s="6"/>
       <c r="T37" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5">
       <c r="A38" s="8"/>
       <c r="B38" s="8"/>
       <c r="C38" s="6"/>
@@ -2086,7 +2077,7 @@
       <c r="S38" s="6"/>
       <c r="T38" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5">
       <c r="A39" s="8"/>
       <c r="B39" s="8"/>
       <c r="C39" s="6"/>
@@ -2108,7 +2099,7 @@
       <c r="S39" s="6"/>
       <c r="T39" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="19.5">
       <c r="A40" s="8"/>
       <c r="B40" s="8"/>
       <c r="C40" s="6"/>
@@ -2130,7 +2121,7 @@
       <c r="S40" s="6"/>
       <c r="T40" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="19.5">
       <c r="A41" s="8"/>
       <c r="B41" s="8"/>
       <c r="C41" s="6"/>
@@ -2152,7 +2143,7 @@
       <c r="S41" s="6"/>
       <c r="T41" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="19.5">
       <c r="A42" s="8"/>
       <c r="B42" s="8"/>
       <c r="C42" s="6"/>
@@ -2174,7 +2165,7 @@
       <c r="S42" s="6"/>
       <c r="T42" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="19.5">
       <c r="A43" s="8"/>
       <c r="B43" s="8"/>
       <c r="C43" s="6"/>
@@ -2196,7 +2187,7 @@
       <c r="S43" s="6"/>
       <c r="T43" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="19.5">
       <c r="A44" s="8"/>
       <c r="B44" s="8"/>
       <c r="C44" s="6"/>
@@ -2218,7 +2209,7 @@
       <c r="S44" s="6"/>
       <c r="T44" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="19.5">
       <c r="A45" s="8"/>
       <c r="B45" s="8"/>
       <c r="C45" s="6"/>

</xml_diff>